<commit_message>
major update. made script that automatically generates shacl file en ontology
</commit_message>
<xml_diff>
--- a/application-profile/application_profile.xlsx
+++ b/application-profile/application_profile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/h.j.m.tummers/git_programming/agriculture-image-metadata/application-profile/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2AC4F36-068C-1347-B672-F60E4994FC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495428FA-60CE-6942-A6B5-08D7628F2247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17280" yWindow="680" windowWidth="21360" windowHeight="20000" xr2:uid="{E7C87683-5EEC-A142-951F-A775E2583B85}"/>
+    <workbookView xWindow="16320" yWindow="3840" windowWidth="21360" windowHeight="20000" xr2:uid="{E7C87683-5EEC-A142-951F-A775E2583B85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="267">
   <si>
     <t>entity</t>
   </si>
@@ -143,15 +143,9 @@
     <t>pixelSize</t>
   </si>
   <si>
-    <t>http://qudt.org/vocab/quantitykind/Length</t>
-  </si>
-  <si>
     <t>xsd:float</t>
   </si>
   <si>
-    <t>http://qudt.org/vocab/unit/MicroM</t>
-  </si>
-  <si>
     <t>focalLength</t>
   </si>
   <si>
@@ -161,9 +155,6 @@
     <t>Focal length of the lens in [mm]</t>
   </si>
   <si>
-    <t>http://qudt.org/vocab/unit/MilliM</t>
-  </si>
-  <si>
     <t>subjectDistance</t>
   </si>
   <si>
@@ -188,9 +179,6 @@
     <t>Spectral band captured by the camera (e.g., RGB, BGR, NIR, Thermal)</t>
   </si>
   <si>
-    <t>RGB</t>
-  </si>
-  <si>
     <t>['rgb', 'nir', 'mono', 'thermal', 'multispectral', 'depth']</t>
   </si>
   <si>
@@ -497,9 +485,6 @@
     <t>ISO-8601 timestamp of image (YYYYMMDDTHHMMSSZmilliseconds 20250917T134658Z)</t>
   </si>
   <si>
-    <t>20251014T093010Z857</t>
-  </si>
-  <si>
     <t>Identifier of the camera that captured the image</t>
   </si>
   <si>
@@ -680,9 +665,6 @@
     <t>Non-crop surface cover visible in the images</t>
   </si>
   <si>
-    <t>['SHELLS', 'STRAW']</t>
-  </si>
-  <si>
     <t>Camera</t>
   </si>
   <si>
@@ -701,30 +683,15 @@
     <t>Plot</t>
   </si>
   <si>
-    <t>hasplot</t>
-  </si>
-  <si>
     <t xml:space="preserve">Images belonging to dataset </t>
   </si>
   <si>
-    <t>Pixel size of sensor in [um] Value is numeric only; unit is defined in separate field."</t>
-  </si>
-  <si>
     <t>https://gd.eppo.int/taxon/</t>
   </si>
   <si>
     <t>xsd:datetime</t>
   </si>
   <si>
-    <t>newont:plot</t>
-  </si>
-  <si>
-    <t>newont:platform</t>
-  </si>
-  <si>
-    <t>newont:image</t>
-  </si>
-  <si>
     <t>xsd:dateTime</t>
   </si>
   <si>
@@ -734,18 +701,12 @@
     <t>Platform</t>
   </si>
   <si>
-    <t>newont:Sensor</t>
-  </si>
-  <si>
     <t>Sensor</t>
   </si>
   <si>
     <t>hasCamera</t>
   </si>
   <si>
-    <t>newont:Camera</t>
-  </si>
-  <si>
     <t>['FLASH', 'DAYLIGHT', ...]</t>
   </si>
   <si>
@@ -758,12 +719,6 @@
     <t>https://example.org/agent/bart-van-marrewijk</t>
   </si>
   <si>
-    <t>example = https://example.org/plot/plot123</t>
-  </si>
-  <si>
-    <t>newont:Crop</t>
-  </si>
-  <si>
     <t>2025-10-14T09:30:10.857Z</t>
   </si>
   <si>
@@ -804,9 +759,6 @@
   </si>
   <si>
     <t>https://w3id.org/agri-image/weed</t>
-  </si>
-  <si>
-    <t>https://w3id.org/agri-images/crop</t>
   </si>
   <si>
     <t>https://w3id.org/agri-image/cameraBox</t>
@@ -841,6 +793,51 @@
   </si>
   <si>
     <t>Crop timing event (e.g., planting, harvesting, flowering, etc.)</t>
+  </si>
+  <si>
+    <t>https://w3id.org/agri-image/pixelSize</t>
+  </si>
+  <si>
+    <t>xsd:decimal</t>
+  </si>
+  <si>
+    <t>SHELLS</t>
+  </si>
+  <si>
+    <t>hasPlot</t>
+  </si>
+  <si>
+    <t>Physical size of one pixel on a sensor, in micrometers</t>
+  </si>
+  <si>
+    <t>https://qudt.org/vocab/unit/MicroM</t>
+  </si>
+  <si>
+    <t>https://qudt.org/vocab/unit/MilliM</t>
+  </si>
+  <si>
+    <t>rgb</t>
+  </si>
+  <si>
+    <t>https://w3id.org/agri-image/crop</t>
+  </si>
+  <si>
+    <t>agimage:plot</t>
+  </si>
+  <si>
+    <t>agimage:platform</t>
+  </si>
+  <si>
+    <t>agimage:image</t>
+  </si>
+  <si>
+    <t>agimage:sensor</t>
+  </si>
+  <si>
+    <t>agimage:camera</t>
+  </si>
+  <si>
+    <t>agimage:crop</t>
   </si>
 </sst>
 </file>
@@ -896,7 +893,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -906,6 +903,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1264,8 +1265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8206725-16E2-CC44-A85F-8143EC23DE3A}">
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1322,7 +1323,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -1351,7 +1352,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -1380,7 +1381,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
@@ -1409,7 +1410,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
@@ -1438,7 +1439,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>
@@ -1467,7 +1468,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B7" t="s">
         <v>31</v>
@@ -1496,19 +1497,19 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B8" t="s">
         <v>34</v>
       </c>
-      <c r="C8" t="s">
-        <v>35</v>
+      <c r="C8" s="5" t="s">
+        <v>252</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>253</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1517,62 +1518,62 @@
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>223</v>
+        <v>256</v>
       </c>
       <c r="I8">
         <v>3.45</v>
       </c>
-      <c r="L8" t="s">
-        <v>37</v>
+      <c r="L8" s="4" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
         <v>38</v>
-      </c>
-      <c r="C9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9" t="s">
-        <v>40</v>
       </c>
       <c r="I9">
         <v>6</v>
       </c>
-      <c r="L9" t="s">
-        <v>41</v>
+      <c r="L9" s="4" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1581,62 +1582,62 @@
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I10">
         <v>400</v>
       </c>
-      <c r="L10" t="s">
-        <v>45</v>
+      <c r="L10" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
         <v>46</v>
       </c>
-      <c r="C11" t="s">
+      <c r="I11" t="s">
+        <v>259</v>
+      </c>
+      <c r="K11" t="s">
         <v>47</v>
-      </c>
-      <c r="D11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11" t="s">
-        <v>49</v>
-      </c>
-      <c r="I11" t="s">
-        <v>50</v>
-      </c>
-      <c r="K11" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="D12" t="s">
         <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1645,24 +1646,24 @@
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D13" t="s">
         <v>4</v>
@@ -1677,21 +1678,21 @@
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="I13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
         <v>20</v>
@@ -1709,21 +1710,21 @@
         <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="D15" t="s">
         <v>4</v>
@@ -1738,18 +1739,18 @@
         <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B16" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="D16" t="s">
         <v>4</v>
@@ -1764,18 +1765,18 @@
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
@@ -1793,22 +1794,22 @@
         <v>1</v>
       </c>
       <c r="H17" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I17" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>210</v>
+      </c>
+      <c r="B18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>224</v>
-      </c>
       <c r="D18" t="s">
         <v>4</v>
       </c>
@@ -1822,21 +1823,21 @@
         <v>1</v>
       </c>
       <c r="H18" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I18" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
@@ -1851,24 +1852,24 @@
         <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I19" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="J19" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
       <c r="D20" t="s">
         <v>4</v>
@@ -1883,24 +1884,24 @@
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J20" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D21" t="s">
         <v>4</v>
@@ -1915,7 +1916,7 @@
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I21">
         <v>60</v>
@@ -1923,13 +1924,13 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D22" t="s">
         <v>4</v>
@@ -1944,7 +1945,7 @@
         <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I22">
         <v>65</v>
@@ -1952,13 +1953,13 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B23" t="s">
-        <v>263</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>266</v>
+        <v>247</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>250</v>
       </c>
       <c r="D23" t="s">
         <v>4</v>
@@ -1970,27 +1971,27 @@
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H23" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B24" t="s">
-        <v>265</v>
+        <v>249</v>
       </c>
       <c r="C24" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D24" t="s">
         <v>4</v>
       </c>
       <c r="E24" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1999,18 +2000,18 @@
         <v>1</v>
       </c>
       <c r="H24" t="s">
-        <v>264</v>
+        <v>248</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B25" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C25" t="s">
         <v>13</v>
@@ -2028,21 +2029,21 @@
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="I25" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C26" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D26" t="s">
         <v>4</v>
@@ -2057,21 +2058,21 @@
         <v>1</v>
       </c>
       <c r="H26" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="I26" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D27" t="s">
         <v>4</v>
@@ -2086,21 +2087,21 @@
         <v>1</v>
       </c>
       <c r="H27" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I27" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B28" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C28" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D28" t="s">
         <v>4</v>
@@ -2115,21 +2116,21 @@
         <v>1</v>
       </c>
       <c r="H28" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I28" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B29" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C29" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D29" t="s">
         <v>4</v>
@@ -2144,7 +2145,7 @@
         <v>1</v>
       </c>
       <c r="H29" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="I29">
         <v>1</v>
@@ -2152,20 +2153,20 @@
     </row>
     <row r="30" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>211</v>
+      </c>
+      <c r="B30" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" t="s">
         <v>217</v>
       </c>
-      <c r="B30" t="s">
-        <v>103</v>
-      </c>
-      <c r="C30" t="s">
-        <v>104</v>
-      </c>
-      <c r="D30" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" t="s">
-        <v>225</v>
-      </c>
       <c r="F30">
         <v>0</v>
       </c>
@@ -2173,28 +2174,28 @@
         <v>1</v>
       </c>
       <c r="H30" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>211</v>
+      </c>
+      <c r="B31" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" t="s">
         <v>217</v>
       </c>
-      <c r="B31" t="s">
-        <v>106</v>
-      </c>
-      <c r="C31" t="s">
-        <v>107</v>
-      </c>
-      <c r="D31" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" t="s">
-        <v>225</v>
-      </c>
       <c r="F31">
         <v>0</v>
       </c>
@@ -2202,28 +2203,28 @@
         <v>1</v>
       </c>
       <c r="H31" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>211</v>
+      </c>
+      <c r="B32" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" t="s">
+        <v>106</v>
+      </c>
+      <c r="D32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" t="s">
         <v>217</v>
       </c>
-      <c r="B32" t="s">
-        <v>109</v>
-      </c>
-      <c r="C32" t="s">
-        <v>110</v>
-      </c>
-      <c r="D32" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" t="s">
-        <v>225</v>
-      </c>
       <c r="F32">
         <v>0</v>
       </c>
@@ -2231,28 +2232,28 @@
         <v>1</v>
       </c>
       <c r="H32" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>211</v>
+      </c>
+      <c r="B33" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" t="s">
+        <v>109</v>
+      </c>
+      <c r="D33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" t="s">
         <v>217</v>
       </c>
-      <c r="B33" t="s">
-        <v>112</v>
-      </c>
-      <c r="C33" t="s">
-        <v>113</v>
-      </c>
-      <c r="D33" t="s">
-        <v>4</v>
-      </c>
-      <c r="E33" t="s">
-        <v>225</v>
-      </c>
       <c r="F33">
         <v>0</v>
       </c>
@@ -2260,21 +2261,21 @@
         <v>1</v>
       </c>
       <c r="H33" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B34" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C34" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D34" t="s">
         <v>4</v>
@@ -2289,79 +2290,79 @@
         <v>1</v>
       </c>
       <c r="H34" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I34" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B35" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C35" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D35" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E35" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="F35">
         <v>1</v>
       </c>
       <c r="G35" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H35" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B36" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C36" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D36" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E36" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="F36">
         <v>0</v>
       </c>
       <c r="G36" t="s">
+        <v>116</v>
+      </c>
+      <c r="H36" t="s">
         <v>120</v>
       </c>
-      <c r="H36" t="s">
-        <v>124</v>
-      </c>
       <c r="I36" s="2" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B37" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C37" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D37" t="s">
         <v>4</v>
@@ -2376,21 +2377,21 @@
         <v>1</v>
       </c>
       <c r="H37" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I37" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B38" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="D38" t="s">
         <v>4</v>
@@ -2405,7 +2406,7 @@
         <v>1</v>
       </c>
       <c r="H38" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="I38">
         <v>15000</v>
@@ -2413,13 +2414,13 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B39" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="D39" t="s">
         <v>4</v>
@@ -2434,7 +2435,7 @@
         <v>1</v>
       </c>
       <c r="H39" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="I39">
         <v>12500</v>
@@ -2442,82 +2443,82 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B40" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="D40" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E40" t="s">
-        <v>226</v>
+        <v>261</v>
       </c>
       <c r="F40">
         <v>1</v>
       </c>
       <c r="G40" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B41" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="D41" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E41" t="s">
-        <v>227</v>
+        <v>262</v>
       </c>
       <c r="F41">
         <v>1</v>
       </c>
       <c r="G41" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B42" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="D42" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E42" t="s">
-        <v>228</v>
+        <v>263</v>
       </c>
       <c r="F42">
         <v>0</v>
       </c>
       <c r="G42" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H42" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B43" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C43" t="s">
         <v>13</v>
@@ -2535,21 +2536,21 @@
         <v>1</v>
       </c>
       <c r="H43" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="I43" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B44" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C44" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D44" t="s">
         <v>4</v>
@@ -2564,76 +2565,74 @@
         <v>1</v>
       </c>
       <c r="H44" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I44" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B45" t="s">
+        <v>135</v>
+      </c>
+      <c r="C45" t="s">
+        <v>136</v>
+      </c>
+      <c r="D45" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" t="s">
+        <v>219</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45" t="s">
+        <v>137</v>
+      </c>
+      <c r="I45" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>212</v>
+      </c>
+      <c r="B46" t="s">
+        <v>255</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D46" t="s">
+        <v>45</v>
+      </c>
+      <c r="E46" t="s">
+        <v>261</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46" t="s">
+        <v>116</v>
+      </c>
+      <c r="H46" t="s">
         <v>139</v>
       </c>
-      <c r="C45" t="s">
-        <v>140</v>
-      </c>
-      <c r="D45" t="s">
-        <v>4</v>
-      </c>
-      <c r="E45" t="s">
-        <v>230</v>
-      </c>
-      <c r="F45">
-        <v>1</v>
-      </c>
-      <c r="G45">
-        <v>1</v>
-      </c>
-      <c r="H45" t="s">
-        <v>141</v>
-      </c>
-      <c r="I45" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>218</v>
-      </c>
-      <c r="B46" t="s">
-        <v>221</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="D46" t="s">
-        <v>48</v>
-      </c>
-      <c r="E46" t="s">
-        <v>226</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-      <c r="G46" t="s">
-        <v>120</v>
-      </c>
-      <c r="H46" t="s">
-        <v>143</v>
-      </c>
-      <c r="I46" s="3" t="s">
-        <v>240</v>
-      </c>
+      <c r="I46" s="8"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B47" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C47" t="s">
         <v>13</v>
@@ -2651,79 +2650,79 @@
         <v>1</v>
       </c>
       <c r="H47" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="I47" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B48" t="s">
+        <v>143</v>
+      </c>
+      <c r="C48" t="s">
+        <v>86</v>
+      </c>
+      <c r="D48" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" t="s">
+        <v>14</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48" t="s">
+        <v>144</v>
+      </c>
+      <c r="I48" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="17" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>213</v>
+      </c>
+      <c r="B49" t="s">
+        <v>146</v>
+      </c>
+      <c r="C49" t="s">
         <v>147</v>
       </c>
-      <c r="C48" t="s">
-        <v>90</v>
-      </c>
-      <c r="D48" t="s">
-        <v>4</v>
-      </c>
-      <c r="E48" t="s">
-        <v>14</v>
-      </c>
-      <c r="F48">
-        <v>0</v>
-      </c>
-      <c r="G48">
-        <v>1</v>
-      </c>
-      <c r="H48" t="s">
+      <c r="D49" t="s">
+        <v>4</v>
+      </c>
+      <c r="E49" t="s">
+        <v>218</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49" t="s">
         <v>148</v>
       </c>
-      <c r="I48" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>219</v>
-      </c>
-      <c r="B49" t="s">
-        <v>150</v>
-      </c>
-      <c r="C49" t="s">
-        <v>151</v>
-      </c>
-      <c r="D49" t="s">
-        <v>4</v>
-      </c>
-      <c r="E49" t="s">
-        <v>229</v>
-      </c>
-      <c r="F49">
-        <v>1</v>
-      </c>
-      <c r="G49">
-        <v>1</v>
-      </c>
-      <c r="H49" t="s">
-        <v>152</v>
-      </c>
-      <c r="I49" t="s">
-        <v>153</v>
+      <c r="I49" s="1" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B50" t="s">
         <v>16</v>
       </c>
       <c r="C50" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D50" t="s">
         <v>4</v>
@@ -2738,7 +2737,7 @@
         <v>1</v>
       </c>
       <c r="H50" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="I50">
         <v>4110035082</v>
@@ -2746,13 +2745,13 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B51" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C51" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D51" t="s">
         <v>4</v>
@@ -2767,21 +2766,21 @@
         <v>1</v>
       </c>
       <c r="H51" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="I51" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B52" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C52" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D52" t="s">
         <v>4</v>
@@ -2796,21 +2795,21 @@
         <v>1</v>
       </c>
       <c r="H52" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="I52" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B53" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C53" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D53" t="s">
         <v>4</v>
@@ -2825,27 +2824,27 @@
         <v>1</v>
       </c>
       <c r="H53" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="I53" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B54" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C54" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D54" t="s">
         <v>4</v>
       </c>
       <c r="E54" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -2854,24 +2853,24 @@
         <v>1</v>
       </c>
       <c r="H54" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="I54">
         <v>0.01</v>
       </c>
       <c r="L54" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B55" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C55" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D55" t="s">
         <v>4</v>
@@ -2886,7 +2885,7 @@
         <v>1</v>
       </c>
       <c r="H55" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="I55">
         <v>1000</v>
@@ -2894,20 +2893,20 @@
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>213</v>
+      </c>
+      <c r="B56" t="s">
+        <v>164</v>
+      </c>
+      <c r="C56" t="s">
+        <v>165</v>
+      </c>
+      <c r="D56" t="s">
+        <v>4</v>
+      </c>
+      <c r="E56" t="s">
         <v>219</v>
       </c>
-      <c r="B56" t="s">
-        <v>169</v>
-      </c>
-      <c r="C56" t="s">
-        <v>170</v>
-      </c>
-      <c r="D56" t="s">
-        <v>4</v>
-      </c>
-      <c r="E56" t="s">
-        <v>230</v>
-      </c>
       <c r="F56">
         <v>0</v>
       </c>
@@ -2915,31 +2914,31 @@
         <v>1</v>
       </c>
       <c r="H56" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="I56" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="L56" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>213</v>
+      </c>
+      <c r="B57" t="s">
+        <v>168</v>
+      </c>
+      <c r="C57" t="s">
+        <v>169</v>
+      </c>
+      <c r="D57" t="s">
+        <v>4</v>
+      </c>
+      <c r="E57" t="s">
         <v>219</v>
       </c>
-      <c r="B57" t="s">
-        <v>173</v>
-      </c>
-      <c r="C57" t="s">
-        <v>174</v>
-      </c>
-      <c r="D57" t="s">
-        <v>4</v>
-      </c>
-      <c r="E57" t="s">
-        <v>230</v>
-      </c>
       <c r="F57">
         <v>0</v>
       </c>
@@ -2947,21 +2946,21 @@
         <v>1</v>
       </c>
       <c r="H57" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="I57" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B58" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C58" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D58" t="s">
         <v>4</v>
@@ -2976,28 +2975,28 @@
         <v>1</v>
       </c>
       <c r="H58" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="I58" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>213</v>
+      </c>
+      <c r="B59" t="s">
+        <v>176</v>
+      </c>
+      <c r="C59" t="s">
+        <v>165</v>
+      </c>
+      <c r="D59" t="s">
+        <v>4</v>
+      </c>
+      <c r="E59" t="s">
         <v>219</v>
       </c>
-      <c r="B59" t="s">
-        <v>181</v>
-      </c>
-      <c r="C59" t="s">
-        <v>170</v>
-      </c>
-      <c r="D59" t="s">
-        <v>4</v>
-      </c>
-      <c r="E59" t="s">
-        <v>230</v>
-      </c>
       <c r="F59">
         <v>1</v>
       </c>
@@ -3005,31 +3004,31 @@
         <v>1</v>
       </c>
       <c r="H59" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="I59" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="L59" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>213</v>
+      </c>
+      <c r="B60" t="s">
+        <v>179</v>
+      </c>
+      <c r="C60" t="s">
+        <v>169</v>
+      </c>
+      <c r="D60" t="s">
+        <v>4</v>
+      </c>
+      <c r="E60" t="s">
         <v>219</v>
       </c>
-      <c r="B60" t="s">
-        <v>184</v>
-      </c>
-      <c r="C60" t="s">
-        <v>174</v>
-      </c>
-      <c r="D60" t="s">
-        <v>4</v>
-      </c>
-      <c r="E60" t="s">
-        <v>230</v>
-      </c>
       <c r="F60">
         <v>1</v>
       </c>
@@ -3037,21 +3036,21 @@
         <v>1</v>
       </c>
       <c r="H60" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="I60" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B61" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C61" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D61" t="s">
         <v>4</v>
@@ -3066,18 +3065,18 @@
         <v>1</v>
       </c>
       <c r="H61" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="I61" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="B62" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C62" t="s">
         <v>13</v>
@@ -3095,21 +3094,21 @@
         <v>1</v>
       </c>
       <c r="H62" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="I62" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="B63" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C63" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D63" t="s">
         <v>4</v>
@@ -3124,67 +3123,67 @@
         <v>1</v>
       </c>
       <c r="H63" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I63" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="B64" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
       <c r="D64" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E64" t="s">
-        <v>232</v>
+        <v>264</v>
       </c>
       <c r="F64">
         <v>0</v>
       </c>
       <c r="G64" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H64" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="B65" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="D65" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E65" t="s">
-        <v>235</v>
+        <v>265</v>
       </c>
       <c r="F65">
         <v>0</v>
       </c>
       <c r="G65" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B66" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C66" t="s">
         <v>13</v>
@@ -3202,21 +3201,21 @@
         <v>1</v>
       </c>
       <c r="H66" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="I66" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B67" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C67" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D67" t="s">
         <v>4</v>
@@ -3231,27 +3230,27 @@
         <v>1</v>
       </c>
       <c r="H67" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="I67" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B68" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C68" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D68" t="s">
         <v>4</v>
       </c>
       <c r="E68" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="F68">
         <v>1</v>
@@ -3260,73 +3259,73 @@
         <v>1</v>
       </c>
       <c r="H68" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="I68" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B69" t="s">
-        <v>199</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>256</v>
+        <v>194</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>260</v>
       </c>
       <c r="D69" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E69" t="s">
-        <v>241</v>
+        <v>266</v>
       </c>
       <c r="F69">
         <v>1</v>
       </c>
       <c r="G69" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H69" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B70" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="D70" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E70" t="s">
-        <v>241</v>
+        <v>266</v>
       </c>
       <c r="F70">
         <v>0</v>
       </c>
       <c r="G70" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H70" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B71" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C71" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D71" t="s">
         <v>4</v>
@@ -3341,21 +3340,21 @@
         <v>1</v>
       </c>
       <c r="H71" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="I71" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B72" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C72" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D72" t="s">
         <v>4</v>
@@ -3370,21 +3369,21 @@
         <v>1</v>
       </c>
       <c r="H72" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I72" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B73" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C73" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D73" t="s">
         <v>4</v>
@@ -3399,20 +3398,22 @@
         <v>1</v>
       </c>
       <c r="H73" t="s">
-        <v>213</v>
-      </c>
-      <c r="I73" t="s">
-        <v>214</v>
+        <v>208</v>
+      </c>
+      <c r="I73" s="7" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C46" r:id="rId1" xr:uid="{2E9A5B41-AC4A-5644-8FA6-C350E4A409CA}"/>
-    <hyperlink ref="C23" r:id="rId2" xr:uid="{8CC53DF7-78CE-4743-80B2-57B93C8631C9}"/>
+    <hyperlink ref="L8" r:id="rId1" xr:uid="{60B0C175-A8BB-1643-950D-B7420F5480F1}"/>
+    <hyperlink ref="L9" r:id="rId2" xr:uid="{E235C97C-715D-BE4C-86AC-91994CDD36BE}"/>
+    <hyperlink ref="L10" r:id="rId3" xr:uid="{3A775AC3-4596-694C-BCE8-C4708D3E823A}"/>
+    <hyperlink ref="C69" r:id="rId4" xr:uid="{1E4E8584-7974-E942-8067-E61B084F7320}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
field fix, removed list of bbox and surfaceLayer *
</commit_message>
<xml_diff>
--- a/application-profile/application_profile.xlsx
+++ b/application-profile/application_profile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/h.j.m.tummers/git_programming/agriculture-image-metadata/application-profile/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\PSG\GlastuinbouwProjecten\418_RoboticaEnAutomatisering\Marrewijk, Bart\usefull_code\python\agriculture-image-metadata\application-profile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495428FA-60CE-6942-A6B5-08D7628F2247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B302823-684B-4A71-B553-FDD0E603760C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16320" yWindow="3840" windowWidth="21360" windowHeight="20000" xr2:uid="{E7C87683-5EEC-A142-951F-A775E2583B85}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{E7C87683-5EEC-A142-951F-A775E2583B85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="268">
   <si>
     <t>entity</t>
   </si>
@@ -450,9 +450,6 @@
   </si>
   <si>
     <t>Field polygon as WKT literal (dcterms:Location)</t>
-  </si>
-  <si>
-    <t>['POLYGON((3.053 47.975, 7.24 47.975, 7.24 53.504, 3.053 53.504, 3.053 47.975))']</t>
   </si>
   <si>
     <t>List of plots in the field</t>
@@ -838,13 +835,19 @@
   </si>
   <si>
     <t>agimage:crop</t>
+  </si>
+  <si>
+    <t>POLYGON((3.053 47.975, 7.24 47.975, 7.24 53.504, 3.053 53.504, 3.053 47.975))'</t>
+  </si>
+  <si>
+    <t>agimage:field</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1265,17 +1268,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8206725-16E2-CC44-A85F-8143EC23DE3A}">
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="89" workbookViewId="0">
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" customWidth="1"/>
+    <col min="6" max="6" width="15.25" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="36.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="39.5" bestFit="1" customWidth="1"/>
@@ -1283,7 +1286,7 @@
     <col min="11" max="11" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1321,9 +1324,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -1350,9 +1353,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -1379,9 +1382,9 @@
         <v>4110035082</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
@@ -1408,9 +1411,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
@@ -1437,9 +1440,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B6" t="s">
         <v>27</v>
@@ -1466,9 +1469,9 @@
         <v>2464</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B7" t="s">
         <v>31</v>
@@ -1495,22 +1498,22 @@
         <v>2056</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B8" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
         <v>252</v>
       </c>
-      <c r="D8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" t="s">
-        <v>253</v>
-      </c>
       <c r="F8">
         <v>1</v>
       </c>
@@ -1518,18 +1521,18 @@
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I8">
         <v>3.45</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B9" t="s">
         <v>36</v>
@@ -1556,12 +1559,12 @@
         <v>6</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B10" t="s">
         <v>39</v>
@@ -1591,9 +1594,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B11" t="s">
         <v>43</v>
@@ -1617,21 +1620,21 @@
         <v>46</v>
       </c>
       <c r="I11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B12" t="s">
         <v>48</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D12" t="s">
         <v>4</v>
@@ -1655,9 +1658,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="20.25">
       <c r="A13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B13" t="s">
         <v>52</v>
@@ -1684,12 +1687,12 @@
         <v>55</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B14" t="s">
         <v>56</v>
@@ -1716,15 +1719,15 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B15" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>242</v>
+      <c r="C15" s="6" t="s">
+        <v>241</v>
       </c>
       <c r="D15" t="s">
         <v>4</v>
@@ -1742,15 +1745,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="31.5">
       <c r="A16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B16" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>243</v>
+      <c r="C16" s="6" t="s">
+        <v>242</v>
       </c>
       <c r="D16" t="s">
         <v>4</v>
@@ -1768,12 +1771,12 @@
         <v>62</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B17" t="s">
         <v>63</v>
@@ -1800,15 +1803,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B18" t="s">
         <v>66</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D18" t="s">
         <v>4</v>
@@ -1829,15 +1832,15 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B19" t="s">
         <v>69</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>244</v>
+      <c r="C19" s="6" t="s">
+        <v>243</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
@@ -1855,21 +1858,21 @@
         <v>70</v>
       </c>
       <c r="I19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J19" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B20" t="s">
         <v>72</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D20" t="s">
         <v>4</v>
@@ -1893,9 +1896,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B21" t="s">
         <v>76</v>
@@ -1922,9 +1925,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B22" t="s">
         <v>79</v>
@@ -1951,15 +1954,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B23" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D23" t="s">
         <v>4</v>
@@ -1974,15 +1977,15 @@
         <v>116</v>
       </c>
       <c r="H23" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B24" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C24" t="s">
         <v>81</v>
@@ -1991,7 +1994,7 @@
         <v>4</v>
       </c>
       <c r="E24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -2000,15 +2003,15 @@
         <v>1</v>
       </c>
       <c r="H24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B25" t="s">
         <v>82</v>
@@ -2035,9 +2038,9 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B26" t="s">
         <v>85</v>
@@ -2064,9 +2067,9 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -2093,9 +2096,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B28" t="s">
         <v>92</v>
@@ -2122,9 +2125,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B29" t="s">
         <v>96</v>
@@ -2151,9 +2154,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B30" t="s">
         <v>99</v>
@@ -2165,7 +2168,7 @@
         <v>4</v>
       </c>
       <c r="E30" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -2177,12 +2180,12 @@
         <v>101</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B31" t="s">
         <v>102</v>
@@ -2194,7 +2197,7 @@
         <v>4</v>
       </c>
       <c r="E31" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -2206,12 +2209,12 @@
         <v>104</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="17" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B32" t="s">
         <v>105</v>
@@ -2223,7 +2226,7 @@
         <v>4</v>
       </c>
       <c r="E32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -2235,12 +2238,12 @@
         <v>107</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="17" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B33" t="s">
         <v>108</v>
@@ -2252,7 +2255,7 @@
         <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -2264,12 +2267,12 @@
         <v>110</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B34" t="s">
         <v>111</v>
@@ -2296,9 +2299,9 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="20.25">
       <c r="A35" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B35" t="s">
         <v>114</v>
@@ -2310,7 +2313,7 @@
         <v>45</v>
       </c>
       <c r="E35" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -2322,12 +2325,12 @@
         <v>117</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="21" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="20.25">
       <c r="A36" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B36" t="s">
         <v>118</v>
@@ -2339,7 +2342,7 @@
         <v>45</v>
       </c>
       <c r="E36" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -2351,12 +2354,12 @@
         <v>120</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B37" t="s">
         <v>121</v>
@@ -2383,15 +2386,15 @@
         <v>124</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B38" t="s">
         <v>125</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D38" t="s">
         <v>4</v>
@@ -2412,15 +2415,15 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B39" t="s">
         <v>127</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>229</v>
+      <c r="C39" s="6" t="s">
+        <v>228</v>
       </c>
       <c r="D39" t="s">
         <v>4</v>
@@ -2441,21 +2444,21 @@
         <v>12500</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B40" t="s">
+        <v>234</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>235</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>236</v>
       </c>
       <c r="D40" t="s">
         <v>45</v>
       </c>
       <c r="E40" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -2464,21 +2467,21 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B41" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D41" t="s">
         <v>45</v>
       </c>
       <c r="E41" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -2487,21 +2490,21 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B42" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D42" t="s">
         <v>45</v>
       </c>
       <c r="E42" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -2510,12 +2513,12 @@
         <v>116</v>
       </c>
       <c r="H42" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B43" t="s">
         <v>129</v>
@@ -2542,9 +2545,9 @@
         <v>131</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B44" t="s">
         <v>132</v>
@@ -2571,9 +2574,9 @@
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B45" t="s">
         <v>135</v>
@@ -2585,7 +2588,7 @@
         <v>4</v>
       </c>
       <c r="E45" t="s">
-        <v>219</v>
+        <v>14</v>
       </c>
       <c r="F45">
         <v>1</v>
@@ -2596,25 +2599,25 @@
       <c r="H45" t="s">
         <v>137</v>
       </c>
-      <c r="I45" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I45" s="7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B46" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D46" t="s">
         <v>45</v>
       </c>
       <c r="E46" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -2623,16 +2626,16 @@
         <v>116</v>
       </c>
       <c r="H46" t="s">
+        <v>138</v>
+      </c>
+      <c r="I46" s="8"/>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" t="s">
+        <v>212</v>
+      </c>
+      <c r="B47" t="s">
         <v>139</v>
-      </c>
-      <c r="I46" s="8"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>213</v>
-      </c>
-      <c r="B47" t="s">
-        <v>140</v>
       </c>
       <c r="C47" t="s">
         <v>13</v>
@@ -2650,18 +2653,18 @@
         <v>1</v>
       </c>
       <c r="H47" t="s">
+        <v>140</v>
+      </c>
+      <c r="I47" t="s">
         <v>141</v>
       </c>
-      <c r="I47" t="s">
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" t="s">
+        <v>212</v>
+      </c>
+      <c r="B48" t="s">
         <v>142</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>213</v>
-      </c>
-      <c r="B48" t="s">
-        <v>143</v>
       </c>
       <c r="C48" t="s">
         <v>86</v>
@@ -2679,44 +2682,44 @@
         <v>1</v>
       </c>
       <c r="H48" t="s">
+        <v>143</v>
+      </c>
+      <c r="I48" t="s">
         <v>144</v>
       </c>
-      <c r="I48" t="s">
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" t="s">
+        <v>212</v>
+      </c>
+      <c r="B49" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" ht="17" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>213</v>
-      </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>146</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
+        <v>4</v>
+      </c>
+      <c r="E49" t="s">
+        <v>217</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49" t="s">
         <v>147</v>
       </c>
-      <c r="D49" t="s">
-        <v>4</v>
-      </c>
-      <c r="E49" t="s">
-        <v>218</v>
-      </c>
-      <c r="F49">
-        <v>1</v>
-      </c>
-      <c r="G49">
-        <v>1</v>
-      </c>
-      <c r="H49" t="s">
-        <v>148</v>
-      </c>
       <c r="I49" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
       <c r="A50" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B50" t="s">
         <v>16</v>
@@ -2737,15 +2740,15 @@
         <v>1</v>
       </c>
       <c r="H50" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I50">
         <v>4110035082</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12">
       <c r="A51" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B51" t="s">
         <v>132</v>
@@ -2766,18 +2769,18 @@
         <v>1</v>
       </c>
       <c r="H51" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I51" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12">
       <c r="A52" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B52" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C52" t="s">
         <v>86</v>
@@ -2795,18 +2798,18 @@
         <v>1</v>
       </c>
       <c r="H52" t="s">
+        <v>151</v>
+      </c>
+      <c r="I52" t="s">
         <v>152</v>
       </c>
-      <c r="I52" t="s">
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" t="s">
+        <v>212</v>
+      </c>
+      <c r="B53" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>213</v>
-      </c>
-      <c r="B53" t="s">
-        <v>154</v>
       </c>
       <c r="C53" t="s">
         <v>86</v>
@@ -2824,21 +2827,21 @@
         <v>1</v>
       </c>
       <c r="H53" t="s">
+        <v>154</v>
+      </c>
+      <c r="I53" t="s">
         <v>155</v>
       </c>
-      <c r="I53" t="s">
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" t="s">
+        <v>212</v>
+      </c>
+      <c r="B54" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>213</v>
-      </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>157</v>
-      </c>
-      <c r="C54" t="s">
-        <v>158</v>
       </c>
       <c r="D54" t="s">
         <v>4</v>
@@ -2853,24 +2856,24 @@
         <v>1</v>
       </c>
       <c r="H54" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I54">
         <v>0.01</v>
       </c>
       <c r="L54" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55" t="s">
+        <v>212</v>
+      </c>
+      <c r="B55" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>213</v>
-      </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>161</v>
-      </c>
-      <c r="C55" t="s">
-        <v>162</v>
       </c>
       <c r="D55" t="s">
         <v>4</v>
@@ -2885,198 +2888,198 @@
         <v>1</v>
       </c>
       <c r="H55" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I55">
         <v>1000</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12">
       <c r="A56" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B56" t="s">
+        <v>163</v>
+      </c>
+      <c r="C56" t="s">
         <v>164</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
+        <v>4</v>
+      </c>
+      <c r="E56" t="s">
+        <v>218</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56" t="s">
         <v>165</v>
       </c>
-      <c r="D56" t="s">
-        <v>4</v>
-      </c>
-      <c r="E56" t="s">
-        <v>219</v>
-      </c>
-      <c r="F56">
-        <v>0</v>
-      </c>
-      <c r="G56">
-        <v>1</v>
-      </c>
-      <c r="H56" t="s">
+      <c r="I56" t="s">
         <v>166</v>
-      </c>
-      <c r="I56" t="s">
-        <v>167</v>
       </c>
       <c r="L56" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12">
       <c r="A57" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B57" t="s">
+        <v>167</v>
+      </c>
+      <c r="C57" t="s">
         <v>168</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
+        <v>4</v>
+      </c>
+      <c r="E57" t="s">
+        <v>218</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57" t="s">
         <v>169</v>
       </c>
-      <c r="D57" t="s">
-        <v>4</v>
-      </c>
-      <c r="E57" t="s">
-        <v>219</v>
-      </c>
-      <c r="F57">
-        <v>0</v>
-      </c>
-      <c r="G57">
-        <v>1</v>
-      </c>
-      <c r="H57" t="s">
+      <c r="I57" t="s">
         <v>170</v>
       </c>
-      <c r="I57" t="s">
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" t="s">
+        <v>212</v>
+      </c>
+      <c r="B58" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>213</v>
-      </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>172</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
+        <v>4</v>
+      </c>
+      <c r="E58" t="s">
+        <v>14</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58" t="s">
         <v>173</v>
       </c>
-      <c r="D58" t="s">
-        <v>4</v>
-      </c>
-      <c r="E58" t="s">
-        <v>14</v>
-      </c>
-      <c r="F58">
-        <v>0</v>
-      </c>
-      <c r="G58">
-        <v>1</v>
-      </c>
-      <c r="H58" t="s">
+      <c r="I58" t="s">
         <v>174</v>
       </c>
-      <c r="I58" t="s">
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59" t="s">
+        <v>212</v>
+      </c>
+      <c r="B59" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>213</v>
-      </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
+        <v>164</v>
+      </c>
+      <c r="D59" t="s">
+        <v>4</v>
+      </c>
+      <c r="E59" t="s">
+        <v>218</v>
+      </c>
+      <c r="F59">
+        <v>1</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59" t="s">
         <v>176</v>
       </c>
-      <c r="C59" t="s">
-        <v>165</v>
-      </c>
-      <c r="D59" t="s">
-        <v>4</v>
-      </c>
-      <c r="E59" t="s">
-        <v>219</v>
-      </c>
-      <c r="F59">
-        <v>1</v>
-      </c>
-      <c r="G59">
-        <v>1</v>
-      </c>
-      <c r="H59" t="s">
+      <c r="I59" t="s">
         <v>177</v>
-      </c>
-      <c r="I59" t="s">
-        <v>178</v>
       </c>
       <c r="L59" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12">
       <c r="A60" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B60" t="s">
+        <v>178</v>
+      </c>
+      <c r="C60" t="s">
+        <v>168</v>
+      </c>
+      <c r="D60" t="s">
+        <v>4</v>
+      </c>
+      <c r="E60" t="s">
+        <v>218</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60" t="s">
         <v>179</v>
       </c>
-      <c r="C60" t="s">
-        <v>169</v>
-      </c>
-      <c r="D60" t="s">
-        <v>4</v>
-      </c>
-      <c r="E60" t="s">
+      <c r="I60" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" t="s">
+        <v>212</v>
+      </c>
+      <c r="B61" t="s">
+        <v>180</v>
+      </c>
+      <c r="C61" t="s">
+        <v>172</v>
+      </c>
+      <c r="D61" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61" t="s">
+        <v>14</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61" t="s">
+        <v>181</v>
+      </c>
+      <c r="I61" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" t="s">
         <v>219</v>
       </c>
-      <c r="F60">
-        <v>1</v>
-      </c>
-      <c r="G60">
-        <v>1</v>
-      </c>
-      <c r="H60" t="s">
-        <v>180</v>
-      </c>
-      <c r="I60" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>213</v>
-      </c>
-      <c r="B61" t="s">
-        <v>181</v>
-      </c>
-      <c r="C61" t="s">
-        <v>173</v>
-      </c>
-      <c r="D61" t="s">
-        <v>4</v>
-      </c>
-      <c r="E61" t="s">
-        <v>14</v>
-      </c>
-      <c r="F61">
-        <v>0</v>
-      </c>
-      <c r="G61">
-        <v>1</v>
-      </c>
-      <c r="H61" t="s">
+      <c r="B62" t="s">
         <v>182</v>
-      </c>
-      <c r="I61" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>220</v>
-      </c>
-      <c r="B62" t="s">
-        <v>183</v>
       </c>
       <c r="C62" t="s">
         <v>13</v>
@@ -3094,18 +3097,18 @@
         <v>1</v>
       </c>
       <c r="H62" t="s">
+        <v>183</v>
+      </c>
+      <c r="I62" t="s">
         <v>184</v>
       </c>
-      <c r="I62" t="s">
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63" t="s">
+        <v>219</v>
+      </c>
+      <c r="B63" t="s">
         <v>185</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>220</v>
-      </c>
-      <c r="B63" t="s">
-        <v>186</v>
       </c>
       <c r="C63" t="s">
         <v>86</v>
@@ -3123,27 +3126,27 @@
         <v>1</v>
       </c>
       <c r="H63" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I63" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
       <c r="A64" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B64" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D64" t="s">
         <v>45</v>
       </c>
       <c r="E64" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F64">
         <v>0</v>
@@ -3152,24 +3155,24 @@
         <v>116</v>
       </c>
       <c r="H64" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
       <c r="A65" t="s">
+        <v>220</v>
+      </c>
+      <c r="B65" t="s">
         <v>221</v>
       </c>
-      <c r="B65" t="s">
-        <v>222</v>
-      </c>
       <c r="C65" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D65" t="s">
         <v>45</v>
       </c>
       <c r="E65" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F65">
         <v>0</v>
@@ -3178,12 +3181,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B66" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C66" t="s">
         <v>13</v>
@@ -3201,18 +3204,18 @@
         <v>1</v>
       </c>
       <c r="H66" t="s">
+        <v>189</v>
+      </c>
+      <c r="I66" t="s">
         <v>190</v>
       </c>
-      <c r="I66" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B67" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C67" t="s">
         <v>86</v>
@@ -3230,15 +3233,15 @@
         <v>1</v>
       </c>
       <c r="H67" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I67" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B68" t="s">
         <v>135</v>
@@ -3250,7 +3253,7 @@
         <v>4</v>
       </c>
       <c r="E68" t="s">
-        <v>219</v>
+        <v>14</v>
       </c>
       <c r="F68">
         <v>1</v>
@@ -3259,27 +3262,27 @@
         <v>1</v>
       </c>
       <c r="H68" t="s">
+        <v>192</v>
+      </c>
+      <c r="I68" s="7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" t="s">
+        <v>213</v>
+      </c>
+      <c r="B69" t="s">
         <v>193</v>
       </c>
-      <c r="I68" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>214</v>
-      </c>
-      <c r="B69" t="s">
-        <v>194</v>
-      </c>
       <c r="C69" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D69" t="s">
         <v>45</v>
       </c>
       <c r="E69" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F69">
         <v>1</v>
@@ -3288,24 +3291,24 @@
         <v>116</v>
       </c>
       <c r="H69" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" t="s">
+        <v>213</v>
+      </c>
+      <c r="B70" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>214</v>
-      </c>
-      <c r="B70" t="s">
-        <v>196</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>240</v>
+      <c r="C70" s="6" t="s">
+        <v>239</v>
       </c>
       <c r="D70" t="s">
         <v>45</v>
       </c>
       <c r="E70" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F70">
         <v>0</v>
@@ -3314,94 +3317,94 @@
         <v>116</v>
       </c>
       <c r="H70" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" t="s">
+        <v>213</v>
+      </c>
+      <c r="B71" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>214</v>
-      </c>
-      <c r="B71" t="s">
+      <c r="C71" t="s">
         <v>198</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D71" t="s">
+        <v>4</v>
+      </c>
+      <c r="E71" t="s">
+        <v>14</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="H71" t="s">
         <v>199</v>
       </c>
-      <c r="D71" t="s">
-        <v>4</v>
-      </c>
-      <c r="E71" t="s">
-        <v>14</v>
-      </c>
-      <c r="F71">
-        <v>0</v>
-      </c>
-      <c r="G71">
-        <v>1</v>
-      </c>
-      <c r="H71" t="s">
+      <c r="I71" t="s">
         <v>200</v>
       </c>
-      <c r="I71" t="s">
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" t="s">
+        <v>213</v>
+      </c>
+      <c r="B72" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>214</v>
-      </c>
-      <c r="B72" t="s">
+      <c r="C72" t="s">
         <v>202</v>
       </c>
-      <c r="C72" t="s">
+      <c r="D72" t="s">
+        <v>4</v>
+      </c>
+      <c r="E72" t="s">
+        <v>14</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>1</v>
+      </c>
+      <c r="H72" t="s">
         <v>203</v>
       </c>
-      <c r="D72" t="s">
-        <v>4</v>
-      </c>
-      <c r="E72" t="s">
-        <v>14</v>
-      </c>
-      <c r="F72">
-        <v>0</v>
-      </c>
-      <c r="G72">
-        <v>1</v>
-      </c>
-      <c r="H72" t="s">
+      <c r="I72" t="s">
         <v>204</v>
       </c>
-      <c r="I72" t="s">
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" t="s">
+        <v>213</v>
+      </c>
+      <c r="B73" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>214</v>
-      </c>
-      <c r="B73" t="s">
+      <c r="C73" t="s">
         <v>206</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
+        <v>4</v>
+      </c>
+      <c r="E73" t="s">
+        <v>14</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73" t="s">
+        <v>116</v>
+      </c>
+      <c r="H73" t="s">
         <v>207</v>
       </c>
-      <c r="D73" t="s">
-        <v>4</v>
-      </c>
-      <c r="E73" t="s">
-        <v>14</v>
-      </c>
-      <c r="F73">
-        <v>0</v>
-      </c>
-      <c r="G73">
-        <v>1</v>
-      </c>
-      <c r="H73" t="s">
-        <v>208</v>
-      </c>
       <c r="I73" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -3410,10 +3413,16 @@
     <hyperlink ref="L9" r:id="rId2" xr:uid="{E235C97C-715D-BE4C-86AC-91994CDD36BE}"/>
     <hyperlink ref="L10" r:id="rId3" xr:uid="{3A775AC3-4596-694C-BCE8-C4708D3E823A}"/>
     <hyperlink ref="C69" r:id="rId4" xr:uid="{1E4E8584-7974-E942-8067-E61B084F7320}"/>
+    <hyperlink ref="C39" r:id="rId5" xr:uid="{F0241949-5C80-4390-9067-F785B017D2E7}"/>
+    <hyperlink ref="C70" r:id="rId6" xr:uid="{4992401C-B193-48E1-8EDF-E958ABCB9A4F}"/>
+    <hyperlink ref="C19" r:id="rId7" xr:uid="{7E180521-A14A-4BE7-8EF7-6E876FED65C5}"/>
+    <hyperlink ref="C8" r:id="rId8" xr:uid="{F1894355-B2E0-4752-90B8-169BD6C2A2D9}"/>
+    <hyperlink ref="C15" r:id="rId9" xr:uid="{896E71B3-D8DA-437F-A483-582780172783}"/>
+    <hyperlink ref="C16" r:id="rId10" xr:uid="{1E9B5684-52FB-471D-BD4D-2470DBA40915}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>